<commit_message>
running generator to see generated files
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rfef451ef2f214db6"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R56481d99bb4c4d57"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -1014,7 +1014,7 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-07-29T00:00:00</x:t>
+          <x:t xml:space="preserve">2023-10-03T00:00:00</x:t>
         </x:is>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
creating demo cred feto
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Re0eb4cb98ca24fe2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R840fa55b7c2b4bda"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -2170,7 +2170,71 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="67">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">BuilderGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/BuilderGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/BuilderGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/MelGrubb/BuilderGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-04T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="68">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CredFetoEnum</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CredFetoEnum</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Credfeto.Enumeration.Source.Generation/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/credfeto/credfeto-enum-source-generation</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Enum</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-05T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F66"/>
+  <x:autoFilter ref="A1:F68"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
trying to make works
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R00ffc5a76d8b4212"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R0eaeece0dab44034"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -2522,7 +2522,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="78">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">DynamicsMapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DynamicsMapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/YC.DynamicsMapper/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/YonatanCohavi/DynamicsMapper/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Mapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-16T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F77"/>
+  <x:autoFilter ref="A1:F78"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add RSCG_UtilityTypes to examples
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R1f35977e493941b7"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R159d14859a4d452e"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3002,7 +3002,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="93">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_UtilityTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_UtilityTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_UtilityTypes/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_UtilityTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-12-22T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F92"/>
+  <x:autoFilter ref="A1:F93"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add HsuSgSync to examples
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rda15df9f67d8446a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rd1e61ebb71734188"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3130,7 +3130,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="97">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">HsuSgSync</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/HsuSgSync</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Hsu.Sg.Sync/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/hsu-net/source-generators</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-10T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F96"/>
+  <x:autoFilter ref="A1:F97"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and add BuildInfo
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rb0b184e5499b4204"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R3ec91e35287b4a80"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3258,7 +3258,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="101">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">BuildInfo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/BuildInfo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/BuildInfo/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/LinkDotNet.BuildInformation</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-20T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F100"/>
+  <x:autoFilter ref="A1:F101"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update code examples with chorn embedded res
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R3ec91e35287b4a80"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Re120034df6104cd3"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3276,7 +3276,7 @@
       </x:c>
       <x:c r="D" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/LinkDotNet.BuildInformation</x:t>
+          <x:t xml:space="preserve">https://github.com/linkdotnet/BuildInformation</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -3290,7 +3290,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="102">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Chorn.EmbeddedResourceAccessGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/EmbedRes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Chorn.EmbeddedResourceAccessGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ChristophHornung/EmbeddedResourceGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FilesToCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-21T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F101"/>
+  <x:autoFilter ref="A1:F102"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add ExcludeDirectoryGenerated property to Data class
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rd7a4c1a748af411f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R72a3cc35afd94145"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -337,7 +337,7 @@
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">EnhancementInterface</x:t>
+          <x:t xml:space="preserve">Interface</x:t>
         </x:is>
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">EnhancementInterface</x:t>
+          <x:t xml:space="preserve">Interface</x:t>
         </x:is>
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">EnhancementInterface</x:t>
+          <x:t xml:space="preserve">Interface</x:t>
         </x:is>
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
@@ -1873,34 +1873,802 @@
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
         <x:is>
+          <x:t xml:space="preserve">Interface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-08-26T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="58">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_Utils_Memo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Memo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/rscgutils</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_Utils</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FunctionalProgramming</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-08-27T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="59">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">ThisAssembly_Resources</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ThisAssembly_Resources</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/ThisAssembly.Resources/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/devlooped/ThisAssembly</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FilesToCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-09-16T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="60">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">SourceGenerator.Helper.CopyCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/SourceGenerator.Helper.CopyCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/SourceGenerator.Helper.CopyCode/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/LokiMidgard/SourceGenerator.Helper.CopyCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-09-17T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="61">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">SafeRouting</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/SafeRouting</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/SafeRouting/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/daviddotcs/safe-routing</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">API</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-09-23T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="62">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">ProtobufSourceGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ProtobufSourceGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/LaDeak.ProtobufSourceGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ladeak/ProtobufSourceGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Serializer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-09-24T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="63">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_Decorator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_Decorator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_Decorator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_Decorator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
           <x:t xml:space="preserve">EnhancementClass</x:t>
         </x:is>
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-08-26T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="58">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">RSCG_Utils_Memo</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Memo</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/rscgutils</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_Utils</x:t>
+          <x:t xml:space="preserve">2023-09-30T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="64">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">StringLiteral</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/StringLiteral</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/StringLiteralGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ufcpp/StringLiteralGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Optimizer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-01T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="65">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">ResXGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ResXGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Aigamo.ResXGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ycanardeau/ResXGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FilesToCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-02T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="66">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Disposer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Disposer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Disposer/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/HakamFostok/Disposer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Disposer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-03T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="67">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">BuilderGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/BuilderGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/BuilderGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/MelGrubb/BuilderGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-04T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="68">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">MapTo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/MapTo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/MapTo/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/mrtaikandi/MapTo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Mapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-05T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="69">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">JsonPolymorphicGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/JsonPolymorphicGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/GoLive.Generator.JsonPolymorphicGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/surgicalcoder/JsonPolymorphicGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Serializer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-06T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="70">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_Templating</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_Templating</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_Templating/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/rscg_templating/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Templating</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-07T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="71">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">MagicMap</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/MagicMap</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/MagicMap/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/bramerdaniel/MagicMap</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Mapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-08T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="72">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">DisposableHelpers</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DisposableHelpers</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/DisposableHelpers/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Kiryuumaru/DisposableHelpers</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Disposer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-09T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="73">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Meziantou.Polyfill</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Poly</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Meziantou.Polyfill/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/meziantou/Meziantou.Polyfill</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-10T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="74">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">IDisposableGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/IDisposableGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/IDisposableGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Elskom/IDisposableGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Disposer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-11T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="75">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CredFetoEnum</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CredFetoEnum</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Credfeto.Enumeration.Source.Generation/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/credfeto/credfeto-enum-source-generation</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Enum</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-12T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="76">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">StaticReflection</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/StaticReflection</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/FastStaticReflection/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Cricle/StaticReflection/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-13T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="77">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">UnitGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/UnitGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/UnitGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Cysharp/UnitGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">PrimitiveObsession</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-15T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="78">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">DynamicsMapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DynamicsMapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/YC.DynamicsMapper/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/YonatanCohavi/DynamicsMapper/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Mapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-16T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="79">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">MinimalApiBuilder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/MinimalApiBuilder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/MinimalApiBuilder/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/JensDll/MinimalApiBuilder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">API</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-26T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="80">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">DudNet</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DudNet</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Jwshyns.DudNet/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/jwshyns/DudNet</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-27T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="81">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AutoConstructor</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AutoConstructor</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/AutoConstructor/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/k94ll13nn3/AutoConstructor</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Constructor</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-28T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="82">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">N.SourceGenerators.UnionTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/N.SourceGenerators.UnionTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/N.SourceGenerators.UnionTypes/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Ne4to/N.SourceGenerators.UnionTypes</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -1910,61 +2678,221 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-08-27T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="59">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">ThisAssembly_Resources</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ThisAssembly_Resources</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/ThisAssembly.Resources/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/devlooped/ThisAssembly</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">FilesToCode</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-09-16T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="60">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">SourceGenerator.Helper.CopyCode</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/SourceGenerator.Helper.CopyCode</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/SourceGenerator.Helper.CopyCode/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/LokiMidgard/SourceGenerator.Helper.CopyCode</x:t>
+          <x:t xml:space="preserve">2023-10-29T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="83">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">jsonConverterSourceGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/jscsg</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Aviationexam.GeneratedJsonConverters.SourceGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/aviationexam/json-converter-source-generator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Serializer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-10-30T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="84">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">PrimaryParameter</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/PrimaryParameter</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/FaustVX.PrimaryParameter.SG</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/FaustVX/PrimaryParameter</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Constructor</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-11-15T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="85">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Biwen.AutoClassGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Biwen.AutoClassGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Biwen.AutoClassGen/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/vipwan/Biwen.AutoClassGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Interface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-11-16T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="86">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Microsoft.Extensions.Options.Generators.OptionsValidatorGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/OptValidator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Options</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/dotnet/runtime</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-11-17T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="87">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Microsoft.Extensions.Configuration.Binder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ConfigBinder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Configuration.Binder/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://learn.microsoft.com/en-us/dotnet/core/whats-new/dotnet-8#configuration-binding-source-generator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">API</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-11-18T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="88">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RDG</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RDG</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Http</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/dotnet/aspnetcore</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">API</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-11-19T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="89">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Com</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/COM</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/System.Runtime.InteropServices/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/dotnet/runtime</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -1974,93 +2902,61 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-09-17T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="61">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">SafeRouting</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/SafeRouting</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/SafeRouting/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/daviddotcs/safe-routing</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">API</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-09-23T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="62">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">ProtobufSourceGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ProtobufSourceGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/LaDeak.ProtobufSourceGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ladeak/ProtobufSourceGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Serializer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-09-24T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="63">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">RSCG_Decorator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_Decorator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_Decorator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_Decorator</x:t>
+          <x:t xml:space="preserve">2023-11-20T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="90">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">InterceptorTemplate</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/InterceptorTemplate</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_InterceptorTemplate/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_InterceptorTemplate</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Templating</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2023-11-29T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="91">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">TelemetryLogging</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/TelemetryLogging</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Telemetry.Abstractions/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/dotnet/extensions</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -2070,125 +2966,29 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-09-30T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="64">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">StringLiteral</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/StringLiteral</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/StringLiteralGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ufcpp/StringLiteralGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Optimizer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-01T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="65">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">ResXGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ResXGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Aigamo.ResXGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ycanardeau/ResXGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">FilesToCode</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-02T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="66">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Disposer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Disposer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Disposer/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/HakamFostok/Disposer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Disposer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-03T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="67">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">BuilderGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/BuilderGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/BuilderGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/MelGrubb/BuilderGenerator</x:t>
+          <x:t xml:space="preserve">2023-11-30T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="92">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Ling.Audit</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Ling.Audit</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Ling.Audit/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ling921/dotnet-lib/</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -2198,189 +2998,29 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-10-04T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="68">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">MapTo</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/MapTo</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/MapTo/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/mrtaikandi/MapTo</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Mapper</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-05T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="69">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">JsonPolymorphicGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/JsonPolymorphicGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/GoLive.Generator.JsonPolymorphicGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/surgicalcoder/JsonPolymorphicGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Serializer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-06T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="70">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">RSCG_Templating</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_Templating</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_Templating/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ignatandrei/rscg_templating/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Templating</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-07T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="71">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">MagicMap</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/MagicMap</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/MagicMap/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/bramerdaniel/MagicMap</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Mapper</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-08T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="72">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">DisposableHelpers</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DisposableHelpers</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/DisposableHelpers/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/Kiryuumaru/DisposableHelpers</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Disposer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-09T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="73">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Meziantou.Polyfill</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Poly</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Meziantou.Polyfill/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/meziantou/Meziantou.Polyfill</x:t>
+          <x:t xml:space="preserve">2023-12-12T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="93">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_UtilityTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_UtilityTypes</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_UtilityTypes/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_UtilityTypes</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -2390,93 +3030,61 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-10-10T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="74">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">IDisposableGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/IDisposableGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/IDisposableGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/Elskom/IDisposableGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Disposer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-11T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="75">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">CredFetoEnum</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CredFetoEnum</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Credfeto.Enumeration.Source.Generation/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/credfeto/credfeto-enum-source-generation</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Enum</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-12T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="76">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">StaticReflection</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/StaticReflection</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/FastStaticReflection/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/Cricle/StaticReflection/</x:t>
+          <x:t xml:space="preserve">2023-12-22T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="94">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">mocklis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Mocklis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/mocklis/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/mocklis/mocklis/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Tests</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-03T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="95">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AspectGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AspectGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/AspectGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/igor-tkachev/AspectGenerator</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -2486,29 +3094,93 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-10-13T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="77">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">UnitGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/UnitGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/UnitGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/Cysharp/UnitGenerator</x:t>
+          <x:t xml:space="preserve">2024-01-07T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="96">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CopyCat</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CopyCat</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Copycat/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Otaman/Copycat/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Interface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-09T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="97">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">HsuSgSync</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/HsuSgSync</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Hsu.Sg.Sync/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/hsu-net/source-generators</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-10T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="98">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">DomainPrimitives</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DomainPrimitives</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/AltaSoft.DomainPrimitives.Generator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/altasoft/DomainPrimitives</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -2518,157 +3190,29 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-10-15T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="78">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">DynamicsMapper</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DynamicsMapper</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/YC.DynamicsMapper/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/YonatanCohavi/DynamicsMapper/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Mapper</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-16T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="79">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">MinimalApiBuilder</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/MinimalApiBuilder</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/MinimalApiBuilder/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/JensDll/MinimalApiBuilder</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">API</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-26T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="80">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">DudNet</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DudNet</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Jwshyns.DudNet/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/jwshyns/DudNet</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-27T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="81">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">AutoConstructor</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AutoConstructor</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/AutoConstructor/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/k94ll13nn3/AutoConstructor</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Constructor</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-28T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="82">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">N.SourceGenerators.UnionTypes</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/N.SourceGenerators.UnionTypes</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/N.SourceGenerators.UnionTypes/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/Ne4to/N.SourceGenerators.UnionTypes</x:t>
+          <x:t xml:space="preserve">2024-01-11T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="99">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Funcky.DiscriminatedUnion</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/FUD</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Funcky.DiscriminatedUnion/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/polyadic/funcky-discriminated-union</x:t>
         </x:is>
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
@@ -2678,550 +3222,6 @@
       </x:c>
       <x:c r="F" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">2023-10-29T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="83">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">jsonConverterSourceGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/jscsg</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Aviationexam.GeneratedJsonConverters.SourceGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/aviationexam/json-converter-source-generator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Serializer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-10-30T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="84">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PrimaryParameter</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/PrimaryParameter</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/FaustVX.PrimaryParameter.SG</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/FaustVX/PrimaryParameter</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Constructor</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-15T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="85">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Biwen.AutoClassGen</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Biwen.AutoClassGen</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Biwen.AutoClassGen/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/vipwan/Biwen.AutoClassGen</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementInterface</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-16T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="86">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Microsoft.Extensions.Options.Generators.OptionsValidatorGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/OptValidator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Options</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/dotnet/runtime</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-17T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="87">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Microsoft.Extensions.Configuration.Binder</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ConfigBinder</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Configuration.Binder/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://learn.microsoft.com/en-us/dotnet/core/whats-new/dotnet-8#configuration-binding-source-generator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">API</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-18T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="88">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">RDG</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RDG</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Http</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/dotnet/aspnetcore</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">API</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-19T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="89">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Com</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/COM</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/System.Runtime.InteropServices/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/dotnet/runtime</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementProject</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-20T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="90">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">InterceptorTemplate</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/InterceptorTemplate</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_InterceptorTemplate/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_InterceptorTemplate</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Templating</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-29T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="91">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">TelemetryLogging</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/TelemetryLogging</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.Extensions.Telemetry.Abstractions/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/dotnet/extensions</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-11-30T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="92">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Ling.Audit</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Ling.Audit</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Ling.Audit/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ling921/dotnet-lib/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-12-12T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="93">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">RSCG_UtilityTypes</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_UtilityTypes</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_UtilityTypes/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_UtilityTypes</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2023-12-22T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="94">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">mocklis</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Mocklis</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/mocklis/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/mocklis/mocklis/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Tests</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2024-01-03T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="95">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">AspectGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AspectGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/AspectGenerator/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/igor-tkachev/AspectGenerator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2024-01-07T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="96">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">CopyCat</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CopyCat</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Copycat/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/Otaman/Copycat/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementInterface</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2024-01-09T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="97">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">HsuSgSync</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/HsuSgSync</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Hsu.Sg.Sync/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/hsu-net/source-generators</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">EnhancementClass</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2024-01-10T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="98">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">DomainPrimitives</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/DomainPrimitives</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/AltaSoft.DomainPrimitives.Generator</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/altasoft/DomainPrimitives</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PrimitiveObsession</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">2024-01-11T00:00:00</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="99">
-      <x:c r="A" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Funcky.DiscriminatedUnion</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/FUD</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Funcky.DiscriminatedUnion/</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">https://github.com/polyadic/funcky-discriminated-union</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E" s="4" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">FunctionalProgramming</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F" s="4" t="inlineStr">
-        <x:is>
           <x:t xml:space="preserve">2024-01-18T00:00:00</x:t>
         </x:is>
       </x:c>
@@ -3249,7 +3249,7 @@
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">EnhancementInterface</x:t>
+          <x:t xml:space="preserve">Interface</x:t>
         </x:is>
       </x:c>
       <x:c r="F" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Add Hangfire category and example
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R6e06f5667f3f4878"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Ree409799991c4ccb"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3354,7 +3354,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="104">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">HangfireRecurringJob</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/HangfireRecurringJob</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/IeuanWalker.Hangfire.RecurringJob/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/IeuanWalker/Hangfire.RecurringJob</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Hangfire</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-25T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F103"/>
+  <x:autoFilter ref="A1:F104"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and add Weave
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R95f095fff1fb46e8"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R44338bf6617b486c"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3418,7 +3418,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="106">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Weave</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/Weave</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Weave/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/otac0n/Weave</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FilesToCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-27T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F105"/>
+  <x:autoFilter ref="A1:F106"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and metadata
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R44338bf6617b486c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R55c4e2ccafcb4038"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3450,7 +3450,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="107">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">WhatIAmDoing</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/WIAD</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_WhatIAmDoing/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_WhatIAmDoing</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AOP</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-28T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F106"/>
+  <x:autoFilter ref="A1:F107"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add CommandLine example to RSCG-Examples
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Re01da7c21fe8466e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Ra4de4345fa7941af"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3514,7 +3514,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="109">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CommandLine</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CommandLine</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/DotMake.CommandLine/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/dotmake-build/command-line</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-11T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F108"/>
+  <x:autoFilter ref="A1:F109"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and documentation
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Ra4de4345fa7941af"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R727747f776cf4a78"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3546,7 +3546,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="110">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FunicularSwitch</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/FunicularSwitch</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/FunicularSwitch.Generators/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/bluehands/Funicular-Switch</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FunctionalProgramming</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-12T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F109"/>
+  <x:autoFilter ref="A1:F110"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor code to improve performance and readability
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R727747f776cf4a78"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R898c7cabe42d4f12"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3578,7 +3578,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="111">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">jab</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/jab</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/jab/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/pakrym/jab</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">DependencyInjection</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-01-30T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F110"/>
+  <x:autoFilter ref="A1:F111"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add UnionsGenerator to RSCG examples
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rd5056f8330af4883"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R9ddbb21eb4e14c66"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3738,7 +3738,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="116">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">UnionsGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/UnionsGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RhoMicro.CodeAnalysis.UnionsGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/PaulBraetz/RhoMicro.CodeAnalysis/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FunctionalProgramming</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-18T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F115"/>
+  <x:autoFilter ref="A1:F116"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add CopyTo example to various documentation files
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rd7ded13940844e3c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R682f7ad195ee4ecb"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3770,7 +3770,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="117">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CopyTo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CopyTo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RhoMicro.CodeAnalysis.CopyToGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/PaulBraetz/RhoMicro.CodeAnalysis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementClass</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-19T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F116"/>
+  <x:autoFilter ref="A1:F117"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and add PlantUmlClassDiagramGenerator
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R8919f9efb13f4549"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R61a78c8495c04cc3"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3802,7 +3802,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="118">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">PlantUmlClassDiagramGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/PlantUmlClassDiagramGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/PlantUmlClassDiagramGenerator.SourceGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/pierre3/PlantUmlClassDiagramGenerator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-20T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F117"/>
+  <x:autoFilter ref="A1:F118"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples count to 118 with rscg wait
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rf893f8f1defd4cc5"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R72b03eedb5914cc4"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3834,7 +3834,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="119">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_Wait</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_Wait</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_WaitAndOptions/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_WaitAndOptions</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-21T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F118"/>
+  <x:autoFilter ref="A1:F119"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and add AutoGen
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rf316911336184b1d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rc00b8d1ecc1243d4"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3866,7 +3866,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="120">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AutoGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AutoGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Antelcat.AutoGen/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/Antelcat/AutoGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Mapper</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-22T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F119"/>
+  <x:autoFilter ref="A1:F120"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and add LingoGen
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rc00b8d1ecc1243d4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R516d9336e0094096"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3898,7 +3898,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="121">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">LingoGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/LingoGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RubenBroere.LingoGen/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/RubenBroere/lingo-gen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FilesToCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-23T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F120"/>
+  <x:autoFilter ref="A1:F121"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples with AutoSpectre generator
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R4c73c27541a84336"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R6282336ff6b44b24"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3930,7 +3930,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="122">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AutoSpectre</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AutoSpectre</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/AutoSpectre.SourceGeneration</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/jeppevammenkristensen/auto-spectre</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-24T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F121"/>
+  <x:autoFilter ref="A1:F122"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add RSCG_JSON2Class example and update file count to 122
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Re51bc0d4e6cb4965"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R9595f13a60544328"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3962,7 +3962,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="123">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">RSCG_JSON2Class</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/RSCG_JSON2Class</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/RSCG_JSON2Class/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ignatandrei/RSCG_JSON2Class</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FilesToCode</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-02-29T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F122"/>
+  <x:autoFilter ref="A1:F123"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update RSCG examples and add CodeAnalysis
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Re65502edd0af4ce3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R0f07307a2f9e4198"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3994,7 +3994,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="124">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CodeAnalysis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/CodeAnalysis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Feast.CodeAnalysis/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/feast107/CodeAnalysis</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CodeToString</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-03-01T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F123"/>
+  <x:autoFilter ref="A1:F124"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update category in RSCG.json and CodeAnalysis.md
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R0f07307a2f9e4198"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R79d8d0eb40284a89"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -1969,7 +1969,7 @@
       </x:c>
       <x:c r="E" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">EnhancementProject</x:t>
+          <x:t xml:space="preserve">CodeToString</x:t>
         </x:is>
       </x:c>
       <x:c r="F" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Update RSCG examples with new generator
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rc735f5763ce9418b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R52f59cf5fadb4770"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -4058,7 +4058,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="126">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AutoInvoke.Generator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AutoInvoke.Generator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/AutoInvoke.Generator/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/LokiMidgard/AutoInvoke.Generator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">EnhancementProject</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-03-03T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F125"/>
+  <x:autoFilter ref="A1:F126"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update Feast.CodeAnalysis to Feast.CodeAnalysis.Literal
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rdab95ec8a07745f8"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Ra59febc62bc44b3f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -4007,7 +4007,7 @@
       </x:c>
       <x:c r="C" s="4" t="inlineStr">
         <x:is>
-          <x:t xml:space="preserve">https://www.nuget.org/packages/Feast.CodeAnalysis/</x:t>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Feast.CodeAnalysis.Literal/</x:t>
         </x:is>
       </x:c>
       <x:c r="D" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Update RSCG examples and generators
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Ra59febc62bc44b3f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R9bb075cb81ba4e59"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -4122,7 +4122,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="128">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">TypeUtilities</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/TypeUtilities</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/TypeUtilities/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/DragonsLord/TypeUtilities</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">FunctionalProgramming</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-03-05T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F127"/>
+  <x:autoFilter ref="A1:F128"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add Actor category to GeneratorData and update examples
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rbc361096ef3640ec"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R93f3005c4419419b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -4570,7 +4570,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="142">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">ActorSrcGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ActorSrcGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/ActorSrcGen/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/aabs/ActorSrcGen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Actor</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2024-05-01T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F141"/>
+  <x:autoFilter ref="A1:F142"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add AutoInterface and ShadowWriterBuilder examples
Added new examples for the AutoInterface and ShadowWriterBuilder Roslyn source code generators, including documentation, example code, and related metadata. Updated README and supporting files to reflect the increase to 207 tested generators and reorganized the 'later' list for clarity.
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R5aa76e1b5dde4f69"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R07f4a91b229e4512"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -6650,7 +6650,71 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="207">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">ShadowWriterBuilder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ShadowWriterBuilder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/ShadowWriter/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/StefanStolz/ShadowWriter</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Builder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-07-24T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="208">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">AutoInterface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/AutoInterface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/AutoInterface/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/BlackWhiteYoshi/AutoInterface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Interface</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-07-25T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F206"/>
+  <x:autoFilter ref="A1:F208"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add ShadowWriterProjectInfo RSCG example
Added the 209th Roslyn Source Code Generator example, ShadowWriterProjectInfo by Stefan Stolz, including documentation, example project, metadata, and updates to lists and category counts. This generator demonstrates generating C# code from project attributes using the ShadowWriter NuGet package.
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R8c6621b6dceb4e78"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R17f0f01441d74c07"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -6746,7 +6746,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="210">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">ShadowWriterProjectInfo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/ShadowWriterProjectInfo</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/ShadowWriter/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/StefanStolz/ShadowWriter</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Builder</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-07-24T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F209"/>
+  <x:autoFilter ref="A1:F210"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
first try for StackXML
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R2d5177daed3a4fbd"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R5e5764c59a7b4800"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -6842,7 +6842,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="213">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">StackXML</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/StackXML</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/StackXML/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/ZingBallyhoo/StackXML</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Serializer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-08-01T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F212"/>
+  <x:autoFilter ref="A1:F213"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add UtilityVerse.Copy and mvvmgen RSCG examples
Added new examples for UtilityVerse.Copy and mvvmgen Roslyn Source Code Generators, including documentation, data, and sample projects. Updated README, book list, generator data, and related site files to reflect the increase to 228 tested generators. Adjusted generator logic and removed outdated 'later' entries.
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R5dadbd4f63ad4474"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R7366469a691f42db"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -7322,7 +7322,71 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="228">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">UtilityVerse.Copy</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/UtilityVerse.Copy</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/UtilityVerse.Copy/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/purkayasta/TheUtilityVerse</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Clone</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-08-15T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="229">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">mvvmgen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/mvvmgen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/mvvmgen/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/thomasclaudiushuber/mvvmgen</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Serializer</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-08-16T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F227"/>
+  <x:autoFilter ref="A1:F229"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add TeCLI RSCG example and update documentation
Added TeCLI as the 238th Roslyn Source Code Generator example, including new example files, documentation, and metadata. Updated README, lists, and category displays to reflect the new entry and its details. Adjusted templates to show NuGet downloads, GitHub stars, and generation dates for each RSCG.
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R0363f43691724bfc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="Rc32580a9fae740fb"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -7674,7 +7674,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="239">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">TeCLI</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/TeCLI</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/TeCLI/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/tyevco/TeCLI</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CommandLine</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-11-07T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F238"/>
+  <x:autoFilter ref="A1:F239"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add XmlCommentGenerator example and documentation
Added XmlCommentGenerator as the 240th Roslyn Source Code Generator example, including new sample project, documentation, and related metadata. Updated README, lists, and category files to reflect the new example and incremented counts. Also fixed a minor link replacement in MultiGeneratorV2.cs.
</commit_message>
<xml_diff>
--- a/v2/rscg_examples_site/static/exports/RSCG.xlsx
+++ b/v2/rscg_examples_site/static/exports/RSCG.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R8e9332aaeb824f8d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSCG" sheetId="1" r:id="R9b2d96b6502a4c65"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -7738,7 +7738,39 @@
         </x:is>
       </x:c>
     </x:row>
+    <x:row r="241">
+      <x:c r="A" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">XmlCommentGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="B" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://ignatandrei.github.io/RSCG_Examples/v2/docs/XmlCommentGenerator</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="C" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://www.nuget.org/packages/Microsoft.AspNetCore.OpenApi/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">https://github.com/dotnet/dotnet/</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="E" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">API</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="F" s="4" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">2025-11-09T00:00:00</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:F240"/>
+  <x:autoFilter ref="A1:F241"/>
 </x:worksheet>
 </file>
</xml_diff>